<commit_message>
40011-40013 excel template 更新
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40011.xlsx
+++ b/PhoenixCI/Excel_Template/40011.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="rpt_future" sheetId="4" r:id="rId1"/>
@@ -3860,7 +3860,7 @@
   </si>
   <si>
     <r>
-      <t>以SMA及MAX計算保證金變動幅度已達</t>
+      <t>以SMA及MAX計算保證金變動幅度均未達</t>
     </r>
     <r>
       <rPr>
@@ -3879,13 +3879,32 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>得調整標準，且進位後金額改變。</t>
+      <t>得調整標準，或雖達得調整標準但進位後金額不變。</t>
     </r>
     <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>以SMA及MAX計算保證金變動幅度均未達</t>
+      <t>以</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>計算保證金變動幅度已達</t>
     </r>
     <r>
       <rPr>
@@ -3904,32 +3923,175 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>得調整標準，或雖達得調整標準但進位後金額不變。</t>
+      <t>得調整標準，且進位後金額改變。</t>
     </r>
     <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>以</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
+      <t>2.參考現貨資料，以EWMA計算之保證金變動幅度已達</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>得調整標準</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>EWMA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>計算保證金變動幅度已達</t>
+      <t>.參考現貨資料，以SMA或MAX計算之保證金變動幅度已達</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>得調整標準</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>.參考期貨資料，以EWMA計算之保證金變動幅度已達</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>得調整標準</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5.參考期貨資料，以SMA或MAX計算之保證金變動幅度已達</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>得調整標準。</t>
+    </r>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>以SMA或MAX計算保證金變動幅度已達</t>
     </r>
     <r>
       <rPr>
@@ -3949,168 +4111,6 @@
         <charset val="136"/>
       </rPr>
       <t>得調整標準，且進位後金額改變。</t>
-    </r>
-    <phoneticPr fontId="42" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>2.參考現貨資料，以EWMA計算之保證金變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>得調整標準</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>。</t>
-    </r>
-    <phoneticPr fontId="42" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.參考現貨資料，以SMA或MAX計算之保證金變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>得調整標準</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>。</t>
-    </r>
-    <phoneticPr fontId="42" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>.參考期貨資料，以EWMA計算之保證金變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>得調整標準</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>。</t>
-    </r>
-    <phoneticPr fontId="42" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>5.參考期貨資料，以SMA或MAX計算之保證金變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>得調整標準。</t>
     </r>
     <phoneticPr fontId="42" type="noConversion"/>
   </si>
@@ -4131,7 +4131,7 @@
     <numFmt numFmtId="183" formatCode="0.000%"/>
     <numFmt numFmtId="184" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5158,6 +5158,9 @@
     <xf numFmtId="176" fontId="29" fillId="3" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -5167,39 +5170,42 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5214,12 +5220,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -6348,11 +6348,11 @@
   </sheetPr>
   <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A107" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A107" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.875" style="62" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="69" customWidth="1"/>
@@ -6369,30 +6369,30 @@
     <col min="14" max="16384" width="9" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="I1" s="210" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I1" s="211" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="210"/>
+      <c r="J1" s="211"/>
       <c r="K1" s="191"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J2" s="199"/>
       <c r="K2" s="200"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J3" s="199"/>
       <c r="K3" s="200"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J4" s="199"/>
       <c r="K4" s="200"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="199"/>
       <c r="K5" s="200"/>
     </row>
-    <row r="6" spans="1:12" s="57" customFormat="1" ht="44.1" customHeight="1">
+    <row r="6" spans="1:12" s="57" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>0</v>
       </c>
@@ -6403,12 +6403,12 @@
       <c r="D6" s="53"/>
       <c r="E6" s="53"/>
       <c r="F6" s="54"/>
-      <c r="G6" s="208"/>
-      <c r="H6" s="209"/>
+      <c r="G6" s="209"/>
+      <c r="H6" s="210"/>
       <c r="I6" s="55"/>
       <c r="J6" s="56"/>
     </row>
-    <row r="7" spans="1:12" s="61" customFormat="1" ht="95.45" customHeight="1">
+    <row r="7" spans="1:12" s="61" customFormat="1" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="58"/>
       <c r="B7" s="59" t="s">
         <v>2</v>
@@ -6440,7 +6440,7 @@
       <c r="K7" s="60"/>
       <c r="L7" s="60"/>
     </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1">
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="63" t="s">
         <v>3</v>
       </c>
@@ -6455,7 +6455,7 @@
       <c r="K8" s="68"/>
       <c r="L8" s="68"/>
     </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1">
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="70" t="s">
         <v>19</v>
       </c>
@@ -6488,7 +6488,7 @@
       <c r="K9" s="68"/>
       <c r="L9" s="68"/>
     </row>
-    <row r="10" spans="1:12" s="57" customFormat="1" ht="30" customHeight="1">
+    <row r="10" spans="1:12" s="57" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="71"/>
       <c r="B10" s="63" t="s">
         <v>4</v>
@@ -6504,7 +6504,7 @@
       <c r="K10" s="68"/>
       <c r="L10" s="68"/>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="63" t="s">
         <v>5</v>
       </c>
@@ -6519,7 +6519,7 @@
       <c r="K11" s="68"/>
       <c r="L11" s="68"/>
     </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1">
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="63" t="s">
         <v>128</v>
       </c>
@@ -6534,7 +6534,7 @@
       <c r="K12" s="68"/>
       <c r="L12" s="68"/>
     </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="63" t="s">
         <v>129</v>
       </c>
@@ -6549,7 +6549,7 @@
       <c r="K13" s="68"/>
       <c r="L13" s="68"/>
     </row>
-    <row r="14" spans="1:12" s="73" customFormat="1" ht="30" customHeight="1">
+    <row r="14" spans="1:12" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="63" t="s">
         <v>20</v>
       </c>
@@ -6564,7 +6564,7 @@
       <c r="K14" s="68"/>
       <c r="L14" s="68"/>
     </row>
-    <row r="15" spans="1:12" s="73" customFormat="1" ht="30" customHeight="1">
+    <row r="15" spans="1:12" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="63" t="s">
         <v>21</v>
       </c>
@@ -6579,7 +6579,7 @@
       <c r="K15" s="68"/>
       <c r="L15" s="68"/>
     </row>
-    <row r="16" spans="1:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="16" spans="1:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="63" t="s">
         <v>167</v>
       </c>
@@ -6594,7 +6594,7 @@
       <c r="K16" s="68"/>
       <c r="L16" s="68"/>
     </row>
-    <row r="17" spans="2:12" s="73" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="2:12" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="63" t="s">
         <v>45</v>
       </c>
@@ -6609,7 +6609,7 @@
       <c r="K17" s="68"/>
       <c r="L17" s="68"/>
     </row>
-    <row r="18" spans="2:12" s="73" customFormat="1" ht="30" customHeight="1">
+    <row r="18" spans="2:12" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="119" t="s">
         <v>46</v>
       </c>
@@ -6624,7 +6624,7 @@
       <c r="K18" s="68"/>
       <c r="L18" s="68"/>
     </row>
-    <row r="19" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="19" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="119" t="s">
         <v>52</v>
       </c>
@@ -6639,7 +6639,7 @@
       <c r="K19" s="68"/>
       <c r="L19" s="68"/>
     </row>
-    <row r="20" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="20" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="119"/>
       <c r="C20" s="122"/>
       <c r="D20" s="123"/>
@@ -6652,7 +6652,7 @@
       <c r="K20" s="68"/>
       <c r="L20" s="68"/>
     </row>
-    <row r="21" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="21" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="119"/>
       <c r="C21" s="122"/>
       <c r="D21" s="123"/>
@@ -6665,7 +6665,7 @@
       <c r="K21" s="68"/>
       <c r="L21" s="68"/>
     </row>
-    <row r="22" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="22" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="119"/>
       <c r="C22" s="122"/>
       <c r="D22" s="123"/>
@@ -6678,7 +6678,7 @@
       <c r="K22" s="68"/>
       <c r="L22" s="68"/>
     </row>
-    <row r="23" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="23" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="119"/>
       <c r="C23" s="122"/>
       <c r="D23" s="123"/>
@@ -6691,7 +6691,7 @@
       <c r="K23" s="68"/>
       <c r="L23" s="68"/>
     </row>
-    <row r="24" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="24" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="119"/>
       <c r="C24" s="122"/>
       <c r="D24" s="123"/>
@@ -6704,7 +6704,7 @@
       <c r="K24" s="68"/>
       <c r="L24" s="68"/>
     </row>
-    <row r="25" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="25" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="119"/>
       <c r="C25" s="122"/>
       <c r="D25" s="123"/>
@@ -6717,7 +6717,7 @@
       <c r="K25" s="68"/>
       <c r="L25" s="68"/>
     </row>
-    <row r="26" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="26" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="119"/>
       <c r="C26" s="122"/>
       <c r="D26" s="123"/>
@@ -6730,7 +6730,7 @@
       <c r="K26" s="68"/>
       <c r="L26" s="68"/>
     </row>
-    <row r="27" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="27" spans="2:12" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="119"/>
       <c r="C27" s="122"/>
       <c r="D27" s="123"/>
@@ -6743,7 +6743,7 @@
       <c r="K27" s="68"/>
       <c r="L27" s="68"/>
     </row>
-    <row r="28" spans="2:12" s="73" customFormat="1" ht="30" customHeight="1">
+    <row r="28" spans="2:12" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="119" t="s">
         <v>53</v>
       </c>
@@ -6758,7 +6758,7 @@
       <c r="K28" s="68"/>
       <c r="L28" s="68"/>
     </row>
-    <row r="29" spans="2:12" ht="30" customHeight="1">
+    <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="75" t="s">
         <v>48</v>
       </c>
@@ -6773,7 +6773,7 @@
       <c r="K29" s="68"/>
       <c r="L29" s="68"/>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="125" t="s">
         <v>54</v>
       </c>
@@ -6783,7 +6783,7 @@
       <c r="F30" s="126"/>
       <c r="G30" s="126"/>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="125" t="s">
         <v>57</v>
       </c>
@@ -6793,7 +6793,7 @@
       <c r="F31" s="126"/>
       <c r="G31" s="126"/>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="129" t="s">
         <v>55</v>
       </c>
@@ -6803,7 +6803,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="2:12" s="78" customFormat="1" ht="18.75">
+    <row r="33" spans="2:12" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B33" s="125" t="s">
         <v>56</v>
       </c>
@@ -6817,7 +6817,7 @@
       <c r="K33" s="79"/>
       <c r="L33" s="79"/>
     </row>
-    <row r="34" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="34" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="77"/>
       <c r="C34" s="69"/>
       <c r="D34" s="69"/>
@@ -6829,7 +6829,7 @@
       <c r="K34" s="79"/>
       <c r="L34" s="79"/>
     </row>
-    <row r="35" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="35" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="77"/>
       <c r="C35" s="69"/>
       <c r="D35" s="69"/>
@@ -6841,7 +6841,7 @@
       <c r="K35" s="79"/>
       <c r="L35" s="79"/>
     </row>
-    <row r="36" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="36" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="77"/>
       <c r="C36" s="69"/>
       <c r="D36" s="69"/>
@@ -6853,7 +6853,7 @@
       <c r="K36" s="79"/>
       <c r="L36" s="79"/>
     </row>
-    <row r="37" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="37" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="77"/>
       <c r="C37" s="69"/>
       <c r="D37" s="69"/>
@@ -6865,7 +6865,7 @@
       <c r="K37" s="79"/>
       <c r="L37" s="79"/>
     </row>
-    <row r="38" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="38" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="77"/>
       <c r="C38" s="69"/>
       <c r="D38" s="69"/>
@@ -6877,7 +6877,7 @@
       <c r="K38" s="79"/>
       <c r="L38" s="79"/>
     </row>
-    <row r="39" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="39" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="77"/>
       <c r="C39" s="69"/>
       <c r="D39" s="69"/>
@@ -6889,7 +6889,7 @@
       <c r="K39" s="79"/>
       <c r="L39" s="79"/>
     </row>
-    <row r="40" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="40" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="77"/>
       <c r="C40" s="69"/>
       <c r="D40" s="69"/>
@@ -6901,7 +6901,7 @@
       <c r="K40" s="79"/>
       <c r="L40" s="79"/>
     </row>
-    <row r="41" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="41" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="77"/>
       <c r="C41" s="69"/>
       <c r="D41" s="69"/>
@@ -6913,7 +6913,7 @@
       <c r="K41" s="79"/>
       <c r="L41" s="79"/>
     </row>
-    <row r="42" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="42" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="77"/>
       <c r="C42" s="69"/>
       <c r="D42" s="69"/>
@@ -6925,7 +6925,7 @@
       <c r="K42" s="79"/>
       <c r="L42" s="79"/>
     </row>
-    <row r="43" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="43" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="77"/>
       <c r="C43" s="69"/>
       <c r="D43" s="69"/>
@@ -6937,7 +6937,7 @@
       <c r="K43" s="79"/>
       <c r="L43" s="79"/>
     </row>
-    <row r="44" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="44" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="77"/>
       <c r="C44" s="69"/>
       <c r="D44" s="69"/>
@@ -6949,7 +6949,7 @@
       <c r="K44" s="79"/>
       <c r="L44" s="79"/>
     </row>
-    <row r="45" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="45" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="77"/>
       <c r="C45" s="69"/>
       <c r="D45" s="69"/>
@@ -6961,7 +6961,7 @@
       <c r="K45" s="79"/>
       <c r="L45" s="79"/>
     </row>
-    <row r="46" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1">
+    <row r="46" spans="2:12" s="78" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="77"/>
       <c r="C46" s="69"/>
       <c r="D46" s="69"/>
@@ -6973,7 +6973,7 @@
       <c r="K46" s="79"/>
       <c r="L46" s="79"/>
     </row>
-    <row r="47" spans="2:12" s="78" customFormat="1" ht="18.75">
+    <row r="47" spans="2:12" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B47" s="77"/>
       <c r="C47" s="69"/>
       <c r="D47" s="69"/>
@@ -6985,7 +6985,7 @@
       <c r="K47" s="79"/>
       <c r="L47" s="79"/>
     </row>
-    <row r="48" spans="2:12" s="78" customFormat="1" ht="18.75">
+    <row r="48" spans="2:12" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B48" s="77"/>
       <c r="C48" s="69"/>
       <c r="D48" s="69"/>
@@ -6997,7 +6997,7 @@
       <c r="K48" s="79"/>
       <c r="L48" s="79"/>
     </row>
-    <row r="49" spans="1:12" s="78" customFormat="1" ht="18.75">
+    <row r="49" spans="1:12" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B49" s="77"/>
       <c r="C49" s="69"/>
       <c r="D49" s="69"/>
@@ -7009,7 +7009,7 @@
       <c r="K49" s="79"/>
       <c r="L49" s="79"/>
     </row>
-    <row r="50" spans="1:12" s="80" customFormat="1" ht="44.1" customHeight="1">
+    <row r="50" spans="1:12" s="80" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="51" t="s">
         <v>6</v>
       </c>
@@ -7027,7 +7027,7 @@
       <c r="K50" s="79"/>
       <c r="L50" s="79"/>
     </row>
-    <row r="51" spans="1:12" s="80" customFormat="1" ht="24.4" customHeight="1">
+    <row r="51" spans="1:12" s="80" customFormat="1" ht="24.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="51"/>
       <c r="B51" s="51" t="s">
         <v>156</v>
@@ -7043,7 +7043,7 @@
       <c r="K51" s="79"/>
       <c r="L51" s="79"/>
     </row>
-    <row r="52" spans="1:12" ht="26.25" customHeight="1">
+    <row r="52" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="180" t="s">
         <v>138</v>
       </c>
@@ -7054,7 +7054,7 @@
       <c r="G52" s="84"/>
       <c r="H52" s="85"/>
     </row>
-    <row r="53" spans="1:12" ht="48.95" customHeight="1">
+    <row r="53" spans="1:12" ht="48.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="86" t="s">
         <v>2</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="32.25" customHeight="1">
+    <row r="54" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="63" t="s">
         <v>3</v>
       </c>
@@ -7096,7 +7096,7 @@
       <c r="I54" s="194"/>
       <c r="J54" s="202"/>
     </row>
-    <row r="55" spans="1:12" ht="32.25" hidden="1" customHeight="1">
+    <row r="55" spans="1:12" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="70" t="s">
         <v>19</v>
       </c>
@@ -7109,7 +7109,7 @@
       <c r="I55" s="194"/>
       <c r="J55" s="202"/>
     </row>
-    <row r="56" spans="1:12" ht="32.25" customHeight="1">
+    <row r="56" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="63" t="s">
         <v>4</v>
       </c>
@@ -7122,7 +7122,7 @@
       <c r="I56" s="194"/>
       <c r="J56" s="202"/>
     </row>
-    <row r="57" spans="1:12" ht="32.25" customHeight="1">
+    <row r="57" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="63" t="s">
         <v>5</v>
       </c>
@@ -7135,7 +7135,7 @@
       <c r="I57" s="194"/>
       <c r="J57" s="202"/>
     </row>
-    <row r="58" spans="1:12" ht="32.25" customHeight="1">
+    <row r="58" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="63" t="s">
         <v>128</v>
       </c>
@@ -7148,7 +7148,7 @@
       <c r="I58" s="194"/>
       <c r="J58" s="202"/>
     </row>
-    <row r="59" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="59" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="51"/>
       <c r="B59" s="63" t="s">
         <v>20</v>
@@ -7162,7 +7162,7 @@
       <c r="I59" s="194"/>
       <c r="J59" s="202"/>
     </row>
-    <row r="60" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="60" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="51"/>
       <c r="B60" s="63" t="s">
         <v>21</v>
@@ -7176,7 +7176,7 @@
       <c r="I60" s="194"/>
       <c r="J60" s="202"/>
     </row>
-    <row r="61" spans="1:12" s="95" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="61" spans="1:12" s="95" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="51"/>
       <c r="B61" s="63" t="s">
         <v>166</v>
@@ -7190,7 +7190,7 @@
       <c r="I61" s="195"/>
       <c r="J61" s="203"/>
     </row>
-    <row r="62" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="62" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="51"/>
       <c r="B62" s="63" t="s">
         <v>45</v>
@@ -7204,7 +7204,7 @@
       <c r="I62" s="195"/>
       <c r="J62" s="203"/>
     </row>
-    <row r="63" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="63" spans="1:12" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="51"/>
       <c r="B63" s="119" t="s">
         <v>46</v>
@@ -7218,7 +7218,7 @@
       <c r="I63" s="195"/>
       <c r="J63" s="203"/>
     </row>
-    <row r="64" spans="1:12" s="95" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="64" spans="1:12" s="95" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="51"/>
       <c r="B64" s="119" t="s">
         <v>52</v>
@@ -7232,7 +7232,7 @@
       <c r="I64" s="195"/>
       <c r="J64" s="203"/>
     </row>
-    <row r="65" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="65" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="119"/>
       <c r="C65" s="122"/>
       <c r="D65" s="123"/>
@@ -7245,7 +7245,7 @@
       <c r="K65" s="68"/>
       <c r="L65" s="68"/>
     </row>
-    <row r="66" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="66" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="119"/>
       <c r="C66" s="122"/>
       <c r="D66" s="123"/>
@@ -7258,7 +7258,7 @@
       <c r="K66" s="68"/>
       <c r="L66" s="68"/>
     </row>
-    <row r="67" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="67" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="119"/>
       <c r="C67" s="122"/>
       <c r="D67" s="123"/>
@@ -7271,7 +7271,7 @@
       <c r="K67" s="68"/>
       <c r="L67" s="68"/>
     </row>
-    <row r="68" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="68" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="119"/>
       <c r="C68" s="122"/>
       <c r="D68" s="123"/>
@@ -7284,7 +7284,7 @@
       <c r="K68" s="68"/>
       <c r="L68" s="68"/>
     </row>
-    <row r="69" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="69" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="119"/>
       <c r="C69" s="122"/>
       <c r="D69" s="123"/>
@@ -7297,7 +7297,7 @@
       <c r="K69" s="68"/>
       <c r="L69" s="68"/>
     </row>
-    <row r="70" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="70" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="119"/>
       <c r="C70" s="122"/>
       <c r="D70" s="123"/>
@@ -7310,7 +7310,7 @@
       <c r="K70" s="68"/>
       <c r="L70" s="68"/>
     </row>
-    <row r="71" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="71" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="119"/>
       <c r="C71" s="122"/>
       <c r="D71" s="123"/>
@@ -7323,7 +7323,7 @@
       <c r="K71" s="68"/>
       <c r="L71" s="68"/>
     </row>
-    <row r="72" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="72" spans="1:14" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="119"/>
       <c r="C72" s="122"/>
       <c r="D72" s="123"/>
@@ -7336,7 +7336,7 @@
       <c r="K72" s="68"/>
       <c r="L72" s="68"/>
     </row>
-    <row r="73" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="73" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="51"/>
       <c r="B73" s="119" t="s">
         <v>53</v>
@@ -7350,7 +7350,7 @@
       <c r="I73" s="195"/>
       <c r="J73" s="203"/>
     </row>
-    <row r="74" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="74" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="51"/>
       <c r="B74" s="98"/>
       <c r="C74" s="98"/>
@@ -7362,7 +7362,7 @@
       <c r="I74" s="93"/>
       <c r="J74" s="94"/>
     </row>
-    <row r="75" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="75" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="51"/>
       <c r="B75" s="98"/>
       <c r="C75" s="98"/>
@@ -7374,7 +7374,7 @@
       <c r="I75" s="93"/>
       <c r="J75" s="94"/>
     </row>
-    <row r="76" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="76" spans="1:14" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="51"/>
       <c r="B76" s="97"/>
       <c r="C76" s="98"/>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="K76" s="191"/>
     </row>
-    <row r="77" spans="1:14" s="95" customFormat="1" ht="47.45" customHeight="1">
+    <row r="77" spans="1:14" s="95" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="51"/>
       <c r="B77" s="51"/>
       <c r="C77" s="69"/>
@@ -7398,7 +7398,7 @@
       <c r="E77" s="101"/>
       <c r="F77" s="69"/>
     </row>
-    <row r="78" spans="1:14" s="95" customFormat="1" ht="47.45" customHeight="1">
+    <row r="78" spans="1:14" s="95" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="51"/>
       <c r="B78" s="51"/>
       <c r="C78" s="69"/>
@@ -7406,7 +7406,7 @@
       <c r="E78" s="101"/>
       <c r="F78" s="69"/>
     </row>
-    <row r="79" spans="1:14" s="104" customFormat="1" ht="24.75" customHeight="1">
+    <row r="79" spans="1:14" s="104" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="102"/>
       <c r="B79" s="180" t="s">
         <v>171</v>
@@ -7421,7 +7421,7 @@
       <c r="J79" s="95"/>
       <c r="K79" s="103"/>
     </row>
-    <row r="80" spans="1:14" s="108" customFormat="1" ht="73.5" customHeight="1">
+    <row r="80" spans="1:14" s="108" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="105"/>
       <c r="B80" s="161" t="s">
         <v>2</v>
@@ -7455,7 +7455,7 @@
       <c r="M80" s="106"/>
       <c r="N80" s="107"/>
     </row>
-    <row r="81" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1">
+    <row r="81" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="105"/>
       <c r="B81" s="63" t="s">
         <v>3</v>
@@ -7472,7 +7472,7 @@
       <c r="L81" s="110"/>
       <c r="M81" s="110"/>
     </row>
-    <row r="82" spans="1:13" s="108" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="82" spans="1:13" s="108" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="105"/>
       <c r="B82" s="70" t="s">
         <v>19</v>
@@ -7489,7 +7489,7 @@
       <c r="L82" s="110"/>
       <c r="M82" s="110"/>
     </row>
-    <row r="83" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1">
+    <row r="83" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="105"/>
       <c r="B83" s="63" t="s">
         <v>4</v>
@@ -7506,7 +7506,7 @@
       <c r="L83" s="110"/>
       <c r="M83" s="110"/>
     </row>
-    <row r="84" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1">
+    <row r="84" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="105"/>
       <c r="B84" s="63" t="s">
         <v>5</v>
@@ -7523,7 +7523,7 @@
       <c r="L84" s="110"/>
       <c r="M84" s="110"/>
     </row>
-    <row r="85" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1">
+    <row r="85" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="105"/>
       <c r="B85" s="63" t="s">
         <v>128</v>
@@ -7540,7 +7540,7 @@
       <c r="L85" s="110"/>
       <c r="M85" s="110"/>
     </row>
-    <row r="86" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1">
+    <row r="86" spans="1:13" s="108" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="105"/>
       <c r="B86" s="63" t="s">
         <v>20</v>
@@ -7557,7 +7557,7 @@
       <c r="L86" s="110"/>
       <c r="M86" s="110"/>
     </row>
-    <row r="87" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="87" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="51"/>
       <c r="B87" s="63" t="s">
         <v>21</v>
@@ -7574,7 +7574,7 @@
       <c r="L87" s="110"/>
       <c r="M87" s="110"/>
     </row>
-    <row r="88" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="88" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="51"/>
       <c r="B88" s="63" t="s">
         <v>166</v>
@@ -7591,7 +7591,7 @@
       <c r="L88" s="110"/>
       <c r="M88" s="110"/>
     </row>
-    <row r="89" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="89" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="51"/>
       <c r="B89" s="63" t="s">
         <v>45</v>
@@ -7608,7 +7608,7 @@
       <c r="L89" s="110"/>
       <c r="M89" s="110"/>
     </row>
-    <row r="90" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="90" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="51"/>
       <c r="B90" s="119" t="s">
         <v>46</v>
@@ -7625,7 +7625,7 @@
       <c r="L90" s="110"/>
       <c r="M90" s="110"/>
     </row>
-    <row r="91" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="91" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="51"/>
       <c r="B91" s="119" t="s">
         <v>52</v>
@@ -7642,7 +7642,7 @@
       <c r="L91" s="110"/>
       <c r="M91" s="110"/>
     </row>
-    <row r="92" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="92" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="119"/>
       <c r="C92" s="122"/>
       <c r="D92" s="123"/>
@@ -7655,7 +7655,7 @@
       <c r="K92" s="68"/>
       <c r="L92" s="68"/>
     </row>
-    <row r="93" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="93" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="119"/>
       <c r="C93" s="122"/>
       <c r="D93" s="123"/>
@@ -7668,7 +7668,7 @@
       <c r="K93" s="68"/>
       <c r="L93" s="68"/>
     </row>
-    <row r="94" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="94" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="119"/>
       <c r="C94" s="122"/>
       <c r="D94" s="123"/>
@@ -7681,7 +7681,7 @@
       <c r="K94" s="68"/>
       <c r="L94" s="68"/>
     </row>
-    <row r="95" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="95" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="119"/>
       <c r="C95" s="122"/>
       <c r="D95" s="123"/>
@@ -7694,7 +7694,7 @@
       <c r="K95" s="68"/>
       <c r="L95" s="68"/>
     </row>
-    <row r="96" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="96" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="119"/>
       <c r="C96" s="122"/>
       <c r="D96" s="123"/>
@@ -7707,7 +7707,7 @@
       <c r="K96" s="68"/>
       <c r="L96" s="68"/>
     </row>
-    <row r="97" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="97" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="119"/>
       <c r="C97" s="122"/>
       <c r="D97" s="123"/>
@@ -7720,7 +7720,7 @@
       <c r="K97" s="68"/>
       <c r="L97" s="68"/>
     </row>
-    <row r="98" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="98" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="119"/>
       <c r="C98" s="122"/>
       <c r="D98" s="123"/>
@@ -7733,7 +7733,7 @@
       <c r="K98" s="68"/>
       <c r="L98" s="68"/>
     </row>
-    <row r="99" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="99" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="119"/>
       <c r="C99" s="122"/>
       <c r="D99" s="123"/>
@@ -7746,7 +7746,7 @@
       <c r="K99" s="68"/>
       <c r="L99" s="68"/>
     </row>
-    <row r="100" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="100" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="51"/>
       <c r="B100" s="119" t="s">
         <v>53</v>
@@ -7763,7 +7763,7 @@
       <c r="L100" s="110"/>
       <c r="M100" s="110"/>
     </row>
-    <row r="101" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="101" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="51"/>
       <c r="B101" s="83"/>
       <c r="C101" s="83"/>
@@ -7778,7 +7778,7 @@
       <c r="L101" s="110"/>
       <c r="M101" s="110"/>
     </row>
-    <row r="102" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="102" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="51"/>
       <c r="B102" s="180" t="s">
         <v>172</v>
@@ -7795,7 +7795,7 @@
       <c r="L102" s="110"/>
       <c r="M102" s="110"/>
     </row>
-    <row r="103" spans="1:13" s="108" customFormat="1" ht="55.7" customHeight="1">
+    <row r="103" spans="1:13" s="108" customFormat="1" ht="55.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="51"/>
       <c r="B103" s="161" t="s">
         <v>2</v>
@@ -7828,7 +7828,7 @@
       <c r="L103" s="110"/>
       <c r="M103" s="110"/>
     </row>
-    <row r="104" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="104" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="51"/>
       <c r="B104" s="63" t="s">
         <v>3</v>
@@ -7845,7 +7845,7 @@
       <c r="L104" s="110"/>
       <c r="M104" s="110"/>
     </row>
-    <row r="105" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="105" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="51"/>
       <c r="B105" s="70" t="s">
         <v>19</v>
@@ -7862,7 +7862,7 @@
       <c r="L105" s="110"/>
       <c r="M105" s="110"/>
     </row>
-    <row r="106" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="106" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="51"/>
       <c r="B106" s="63" t="s">
         <v>4</v>
@@ -7879,7 +7879,7 @@
       <c r="L106" s="110"/>
       <c r="M106" s="110"/>
     </row>
-    <row r="107" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="107" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="51"/>
       <c r="B107" s="63" t="s">
         <v>5</v>
@@ -7896,7 +7896,7 @@
       <c r="L107" s="110"/>
       <c r="M107" s="110"/>
     </row>
-    <row r="108" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="108" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="51"/>
       <c r="B108" s="63" t="s">
         <v>128</v>
@@ -7913,7 +7913,7 @@
       <c r="L108" s="110"/>
       <c r="M108" s="110"/>
     </row>
-    <row r="109" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="109" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="51"/>
       <c r="B109" s="63" t="s">
         <v>20</v>
@@ -7930,7 +7930,7 @@
       <c r="L109" s="110"/>
       <c r="M109" s="110"/>
     </row>
-    <row r="110" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="110" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="51"/>
       <c r="B110" s="63" t="s">
         <v>21</v>
@@ -7947,7 +7947,7 @@
       <c r="L110" s="110"/>
       <c r="M110" s="110"/>
     </row>
-    <row r="111" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="111" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="51"/>
       <c r="B111" s="63" t="s">
         <v>166</v>
@@ -7964,7 +7964,7 @@
       <c r="L111" s="110"/>
       <c r="M111" s="110"/>
     </row>
-    <row r="112" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="112" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="51"/>
       <c r="B112" s="63" t="s">
         <v>45</v>
@@ -7981,7 +7981,7 @@
       <c r="L112" s="110"/>
       <c r="M112" s="110"/>
     </row>
-    <row r="113" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="113" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="51"/>
       <c r="B113" s="119" t="s">
         <v>46</v>
@@ -7998,7 +7998,7 @@
       <c r="L113" s="110"/>
       <c r="M113" s="110"/>
     </row>
-    <row r="114" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1">
+    <row r="114" spans="1:13" s="108" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="51"/>
       <c r="B114" s="119" t="s">
         <v>52</v>
@@ -8015,7 +8015,7 @@
       <c r="L114" s="110"/>
       <c r="M114" s="110"/>
     </row>
-    <row r="115" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="115" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="119"/>
       <c r="C115" s="122"/>
       <c r="D115" s="123"/>
@@ -8028,7 +8028,7 @@
       <c r="K115" s="68"/>
       <c r="L115" s="68"/>
     </row>
-    <row r="116" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="116" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="119"/>
       <c r="C116" s="122"/>
       <c r="D116" s="123"/>
@@ -8041,7 +8041,7 @@
       <c r="K116" s="68"/>
       <c r="L116" s="68"/>
     </row>
-    <row r="117" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="117" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="119"/>
       <c r="C117" s="122"/>
       <c r="D117" s="123"/>
@@ -8054,7 +8054,7 @@
       <c r="K117" s="68"/>
       <c r="L117" s="68"/>
     </row>
-    <row r="118" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="118" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="119"/>
       <c r="C118" s="122"/>
       <c r="D118" s="123"/>
@@ -8067,7 +8067,7 @@
       <c r="K118" s="68"/>
       <c r="L118" s="68"/>
     </row>
-    <row r="119" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="119" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="119"/>
       <c r="C119" s="122"/>
       <c r="D119" s="123"/>
@@ -8080,7 +8080,7 @@
       <c r="K119" s="68"/>
       <c r="L119" s="68"/>
     </row>
-    <row r="120" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="120" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="119"/>
       <c r="C120" s="122"/>
       <c r="D120" s="123"/>
@@ -8093,7 +8093,7 @@
       <c r="K120" s="68"/>
       <c r="L120" s="68"/>
     </row>
-    <row r="121" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="121" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="119"/>
       <c r="C121" s="122"/>
       <c r="D121" s="123"/>
@@ -8106,7 +8106,7 @@
       <c r="K121" s="68"/>
       <c r="L121" s="68"/>
     </row>
-    <row r="122" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1">
+    <row r="122" spans="1:13" s="73" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="119"/>
       <c r="C122" s="122"/>
       <c r="D122" s="123"/>
@@ -8119,7 +8119,7 @@
       <c r="K122" s="68"/>
       <c r="L122" s="68"/>
     </row>
-    <row r="123" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="123" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="51"/>
       <c r="B123" s="119" t="s">
         <v>53</v>
@@ -8136,7 +8136,7 @@
       <c r="L123" s="110"/>
       <c r="M123" s="110"/>
     </row>
-    <row r="124" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1">
+    <row r="124" spans="1:13" s="108" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="51"/>
       <c r="B124" s="83"/>
       <c r="C124" s="83"/>
@@ -8151,7 +8151,7 @@
       <c r="L124" s="110"/>
       <c r="M124" s="110"/>
     </row>
-    <row r="125" spans="1:13" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="125" spans="1:13" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="51"/>
       <c r="B125" s="180" t="s">
         <v>173</v>
@@ -8165,7 +8165,7 @@
       <c r="I125" s="85"/>
       <c r="J125" s="94"/>
     </row>
-    <row r="126" spans="1:13" s="95" customFormat="1" ht="39">
+    <row r="126" spans="1:13" s="95" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A126" s="51"/>
       <c r="B126" s="161" t="s">
         <v>2</v>
@@ -8195,7 +8195,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="127" spans="1:13" s="95" customFormat="1" ht="32.25" customHeight="1">
+    <row r="127" spans="1:13" s="95" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="51"/>
       <c r="B127" s="177" t="s">
         <v>24</v>
@@ -8209,7 +8209,7 @@
       <c r="I127" s="194"/>
       <c r="J127" s="202"/>
     </row>
-    <row r="128" spans="1:13" ht="45.2" customHeight="1">
+    <row r="128" spans="1:13" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="51" t="s">
         <v>136</v>
       </c>
@@ -8224,7 +8224,7 @@
       <c r="H128" s="112"/>
       <c r="J128" s="95"/>
     </row>
-    <row r="129" spans="1:10" ht="45.2" customHeight="1">
+    <row r="129" spans="1:10" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="51"/>
       <c r="B129" s="111"/>
       <c r="C129" s="108"/>
@@ -8235,7 +8235,7 @@
       <c r="H129" s="112"/>
       <c r="J129" s="95"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B130" s="130" t="s">
         <v>168</v>
       </c>
@@ -8245,23 +8245,23 @@
       <c r="F130" s="81"/>
       <c r="H130" s="112"/>
     </row>
-    <row r="131" spans="1:10">
-      <c r="A131" s="227">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="208">
         <v>1</v>
       </c>
-      <c r="B131" s="228" t="s">
-        <v>176</v>
-      </c>
-      <c r="C131" s="228"/>
-      <c r="D131" s="228"/>
-      <c r="E131" s="228"/>
-      <c r="F131" s="228"/>
-      <c r="G131" s="228"/>
-      <c r="H131" s="228"/>
-      <c r="I131" s="228"/>
-      <c r="J131" s="228"/>
-    </row>
-    <row r="132" spans="1:10">
+      <c r="B131" s="212" t="s">
+        <v>175</v>
+      </c>
+      <c r="C131" s="212"/>
+      <c r="D131" s="212"/>
+      <c r="E131" s="212"/>
+      <c r="F131" s="212"/>
+      <c r="G131" s="212"/>
+      <c r="H131" s="212"/>
+      <c r="I131" s="212"/>
+      <c r="J131" s="212"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B132" s="114"/>
       <c r="C132" s="115"/>
       <c r="D132" s="81"/>
@@ -8269,7 +8269,7 @@
       <c r="F132" s="81"/>
       <c r="H132" s="112"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B133" s="130" t="s">
         <v>169</v>
       </c>
@@ -8279,28 +8279,28 @@
       <c r="F133" s="81"/>
       <c r="H133" s="112"/>
     </row>
-    <row r="134" spans="1:10">
-      <c r="A134" s="227">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" s="208">
         <v>2</v>
       </c>
-      <c r="B134" s="228" t="s">
-        <v>177</v>
-      </c>
-      <c r="C134" s="228"/>
-      <c r="D134" s="228"/>
-      <c r="E134" s="228"/>
-      <c r="F134" s="228"/>
-      <c r="G134" s="228"/>
-      <c r="H134" s="228"/>
-      <c r="I134" s="228"/>
-      <c r="J134" s="228"/>
-    </row>
-    <row r="135" spans="1:10">
+      <c r="B134" s="212" t="s">
+        <v>176</v>
+      </c>
+      <c r="C134" s="212"/>
+      <c r="D134" s="212"/>
+      <c r="E134" s="212"/>
+      <c r="F134" s="212"/>
+      <c r="G134" s="212"/>
+      <c r="H134" s="212"/>
+      <c r="I134" s="212"/>
+      <c r="J134" s="212"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B135" s="114"/>
       <c r="D135" s="116"/>
       <c r="E135" s="57"/>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B136" s="130" t="s">
         <v>169</v>
       </c>
@@ -8310,29 +8310,29 @@
       <c r="F136" s="81"/>
       <c r="H136" s="112"/>
     </row>
-    <row r="137" spans="1:10">
-      <c r="A137" s="227">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="208">
         <v>3</v>
       </c>
-      <c r="B137" s="228" t="s">
-        <v>175</v>
-      </c>
-      <c r="C137" s="228"/>
-      <c r="D137" s="228"/>
-      <c r="E137" s="228"/>
-      <c r="F137" s="228"/>
-      <c r="G137" s="228"/>
-      <c r="H137" s="228"/>
-      <c r="I137" s="228"/>
-      <c r="J137" s="228"/>
-    </row>
-    <row r="138" spans="1:10">
+      <c r="B137" s="212" t="s">
+        <v>181</v>
+      </c>
+      <c r="C137" s="212"/>
+      <c r="D137" s="212"/>
+      <c r="E137" s="212"/>
+      <c r="F137" s="212"/>
+      <c r="G137" s="212"/>
+      <c r="H137" s="212"/>
+      <c r="I137" s="212"/>
+      <c r="J137" s="212"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B138" s="81"/>
       <c r="D138" s="116"/>
       <c r="E138" s="57"/>
       <c r="G138" s="94"/>
     </row>
-    <row r="139" spans="1:10" ht="37.700000000000003" customHeight="1">
+    <row r="139" spans="1:10" ht="37.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="94" t="s">
         <v>51</v>
       </c>
@@ -8577,11 +8577,11 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A3:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B116" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="B116" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B126" sqref="B126:K126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.125" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="26.625" style="1" customWidth="1"/>
@@ -8598,14 +8598,14 @@
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="188"/>
       <c r="H3" s="173"/>
       <c r="K3" s="173" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="16" customFormat="1" ht="22.5" customHeight="1">
+    <row r="7" spans="1:11" s="16" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
@@ -8619,156 +8619,156 @@
       <c r="G7" s="15"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:11" s="17" customFormat="1" ht="48.95" customHeight="1">
+    <row r="8" spans="1:11" s="17" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="170" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="220" t="s">
+      <c r="C8" s="214" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="221"/>
-      <c r="E8" s="220" t="s">
+      <c r="D8" s="215"/>
+      <c r="E8" s="214" t="s">
         <v>144</v>
       </c>
-      <c r="F8" s="221"/>
-      <c r="G8" s="219" t="s">
+      <c r="F8" s="215"/>
+      <c r="G8" s="218" t="s">
         <v>145</v>
       </c>
-      <c r="H8" s="219"/>
+      <c r="H8" s="218"/>
       <c r="I8" s="7"/>
       <c r="J8" s="40"/>
     </row>
-    <row r="9" spans="1:11" ht="19.899999999999999" customHeight="1">
+    <row r="9" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="215"/>
-      <c r="H9" s="215"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="213"/>
+      <c r="F9" s="213"/>
+      <c r="G9" s="213"/>
+      <c r="H9" s="213"/>
       <c r="I9" s="11"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="10" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="215"/>
-      <c r="H10" s="215"/>
+      <c r="C10" s="213"/>
+      <c r="D10" s="213"/>
+      <c r="E10" s="213"/>
+      <c r="F10" s="213"/>
+      <c r="G10" s="213"/>
+      <c r="H10" s="213"/>
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="11" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="215"/>
-      <c r="D11" s="215"/>
-      <c r="E11" s="215"/>
-      <c r="F11" s="215"/>
-      <c r="G11" s="215"/>
-      <c r="H11" s="215"/>
+      <c r="C11" s="213"/>
+      <c r="D11" s="213"/>
+      <c r="E11" s="213"/>
+      <c r="F11" s="213"/>
+      <c r="G11" s="213"/>
+      <c r="H11" s="213"/>
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="12" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="215"/>
-      <c r="D12" s="215"/>
-      <c r="E12" s="215"/>
-      <c r="F12" s="215"/>
-      <c r="G12" s="215"/>
-      <c r="H12" s="215"/>
+      <c r="C12" s="213"/>
+      <c r="D12" s="213"/>
+      <c r="E12" s="213"/>
+      <c r="F12" s="213"/>
+      <c r="G12" s="213"/>
+      <c r="H12" s="213"/>
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="13" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="215"/>
-      <c r="D13" s="215"/>
-      <c r="E13" s="215"/>
-      <c r="F13" s="215"/>
-      <c r="G13" s="215"/>
-      <c r="H13" s="215"/>
+      <c r="C13" s="213"/>
+      <c r="D13" s="213"/>
+      <c r="E13" s="213"/>
+      <c r="F13" s="213"/>
+      <c r="G13" s="213"/>
+      <c r="H13" s="213"/>
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="14" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="215"/>
-      <c r="D14" s="215"/>
-      <c r="E14" s="215"/>
-      <c r="F14" s="215"/>
-      <c r="G14" s="215"/>
-      <c r="H14" s="215"/>
+      <c r="C14" s="213"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="213"/>
+      <c r="F14" s="213"/>
+      <c r="G14" s="213"/>
+      <c r="H14" s="213"/>
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="15" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="213"/>
-      <c r="D15" s="214"/>
-      <c r="E15" s="213"/>
-      <c r="F15" s="214"/>
-      <c r="G15" s="213"/>
-      <c r="H15" s="214"/>
+      <c r="C15" s="216"/>
+      <c r="D15" s="217"/>
+      <c r="E15" s="216"/>
+      <c r="F15" s="217"/>
+      <c r="G15" s="216"/>
+      <c r="H15" s="217"/>
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="16" spans="1:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="213"/>
-      <c r="D16" s="214"/>
-      <c r="E16" s="215"/>
-      <c r="F16" s="214"/>
-      <c r="G16" s="215"/>
-      <c r="H16" s="214"/>
+      <c r="C16" s="216"/>
+      <c r="D16" s="217"/>
+      <c r="E16" s="213"/>
+      <c r="F16" s="217"/>
+      <c r="G16" s="213"/>
+      <c r="H16" s="217"/>
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="2:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="17" spans="2:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="213"/>
-      <c r="D17" s="214"/>
-      <c r="E17" s="213"/>
-      <c r="F17" s="214"/>
-      <c r="G17" s="213"/>
-      <c r="H17" s="214"/>
+      <c r="C17" s="216"/>
+      <c r="D17" s="217"/>
+      <c r="E17" s="216"/>
+      <c r="F17" s="217"/>
+      <c r="G17" s="216"/>
+      <c r="H17" s="217"/>
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="2:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="18" spans="2:11" s="16" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="213"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="215"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="215"/>
-      <c r="H18" s="214"/>
+      <c r="C18" s="216"/>
+      <c r="D18" s="217"/>
+      <c r="E18" s="213"/>
+      <c r="F18" s="217"/>
+      <c r="G18" s="213"/>
+      <c r="H18" s="217"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="2:11" ht="19.899999999999999" customHeight="1">
+    <row r="19" spans="2:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="48" t="s">
         <v>22</v>
       </c>
@@ -8779,7 +8779,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="2:11" ht="19.899999999999999" customHeight="1">
+    <row r="20" spans="2:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>23</v>
       </c>
@@ -8790,7 +8790,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="21" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="48"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -8800,7 +8800,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="22" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="48"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -8810,7 +8810,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="23" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>161</v>
       </c>
@@ -8822,7 +8822,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="24" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>160</v>
       </c>
@@ -8834,7 +8834,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="25" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="186" t="s">
         <v>133</v>
       </c>
@@ -8846,7 +8846,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="26" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="187" t="s">
         <v>162</v>
       </c>
@@ -8858,7 +8858,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="27" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="187" t="s">
         <v>147</v>
       </c>
@@ -8870,7 +8870,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="2:11" s="19" customFormat="1" ht="60.4" customHeight="1">
+    <row r="28" spans="2:11" s="19" customFormat="1" ht="60.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="185" t="s">
         <v>14</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="29" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="41" t="s">
         <v>17</v>
       </c>
@@ -8918,7 +8918,7 @@
       <c r="J29" s="174"/>
       <c r="K29" s="204"/>
     </row>
-    <row r="30" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="30" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="41" t="s">
         <v>25</v>
       </c>
@@ -8937,7 +8937,7 @@
       <c r="J30" s="174"/>
       <c r="K30" s="205"/>
     </row>
-    <row r="31" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="31" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="41" t="s">
         <v>26</v>
       </c>
@@ -8953,7 +8953,7 @@
       <c r="J31" s="174"/>
       <c r="K31" s="204"/>
     </row>
-    <row r="32" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="32" spans="2:11" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="41" t="s">
         <v>27</v>
       </c>
@@ -8972,7 +8972,7 @@
       <c r="J32" s="174"/>
       <c r="K32" s="205"/>
     </row>
-    <row r="33" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="33" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="41" t="s">
         <v>28</v>
       </c>
@@ -8988,7 +8988,7 @@
       <c r="J33" s="174"/>
       <c r="K33" s="204"/>
     </row>
-    <row r="34" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="34" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="41" t="s">
         <v>29</v>
       </c>
@@ -9007,7 +9007,7 @@
       <c r="J34" s="174"/>
       <c r="K34" s="205"/>
     </row>
-    <row r="35" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="35" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="41" t="s">
         <v>30</v>
       </c>
@@ -9023,7 +9023,7 @@
       <c r="J35" s="174"/>
       <c r="K35" s="204"/>
     </row>
-    <row r="36" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="36" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="41" t="s">
         <v>31</v>
       </c>
@@ -9042,7 +9042,7 @@
       <c r="J36" s="174"/>
       <c r="K36" s="205"/>
     </row>
-    <row r="37" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="37" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="41" t="s">
         <v>32</v>
       </c>
@@ -9058,7 +9058,7 @@
       <c r="J37" s="174"/>
       <c r="K37" s="204"/>
     </row>
-    <row r="38" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="38" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="41" t="s">
         <v>33</v>
       </c>
@@ -9077,7 +9077,7 @@
       <c r="J38" s="174"/>
       <c r="K38" s="205"/>
     </row>
-    <row r="39" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="39" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -9087,7 +9087,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="40" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -9097,7 +9097,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="2:12" s="19" customFormat="1" ht="10.15" customHeight="1">
+    <row r="41" spans="2:12" s="19" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -9107,7 +9107,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="2:12" s="19" customFormat="1">
+    <row r="42" spans="2:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="188"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -9121,7 +9121,7 @@
         <v>資料日期：2011年2月22日</v>
       </c>
     </row>
-    <row r="43" spans="2:12" s="19" customFormat="1" ht="10.15" customHeight="1">
+    <row r="43" spans="2:12" s="19" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="188"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -9132,7 +9132,7 @@
       <c r="I43" s="8"/>
       <c r="K43" s="173"/>
     </row>
-    <row r="44" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="44" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -9142,7 +9142,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="19.899999999999999" customHeight="1">
+    <row r="45" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="129" t="s">
         <v>174</v>
       </c>
@@ -9151,7 +9151,7 @@
       <c r="E45" s="23"/>
       <c r="F45" s="24"/>
     </row>
-    <row r="46" spans="2:12" s="16" customFormat="1" ht="72.75" customHeight="1">
+    <row r="46" spans="2:12" s="16" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>14</v>
       </c>
@@ -9184,7 +9184,7 @@
       </c>
       <c r="L46" s="26"/>
     </row>
-    <row r="47" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="47" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="41" t="s">
         <v>34</v>
       </c>
@@ -9201,7 +9201,7 @@
       <c r="K47" s="204"/>
       <c r="L47" s="27"/>
     </row>
-    <row r="48" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="48" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="41" t="s">
         <v>35</v>
       </c>
@@ -9221,7 +9221,7 @@
       <c r="K48" s="205"/>
       <c r="L48" s="27"/>
     </row>
-    <row r="49" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="49" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="41" t="s">
         <v>36</v>
       </c>
@@ -9238,7 +9238,7 @@
       <c r="K49" s="204"/>
       <c r="L49" s="27"/>
     </row>
-    <row r="50" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="50" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="41" t="s">
         <v>37</v>
       </c>
@@ -9258,7 +9258,7 @@
       <c r="K50" s="205"/>
       <c r="L50" s="27"/>
     </row>
-    <row r="51" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="51" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="41" t="s">
         <v>38</v>
       </c>
@@ -9275,7 +9275,7 @@
       <c r="K51" s="204"/>
       <c r="L51" s="27"/>
     </row>
-    <row r="52" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="52" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="41" t="s">
         <v>39</v>
       </c>
@@ -9295,7 +9295,7 @@
       <c r="K52" s="205"/>
       <c r="L52" s="27"/>
     </row>
-    <row r="53" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="53" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="41" t="s">
         <v>40</v>
       </c>
@@ -9312,7 +9312,7 @@
       <c r="K53" s="204"/>
       <c r="L53" s="27"/>
     </row>
-    <row r="54" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="54" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="41" t="s">
         <v>41</v>
       </c>
@@ -9332,7 +9332,7 @@
       <c r="K54" s="205"/>
       <c r="L54" s="27"/>
     </row>
-    <row r="55" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="55" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="41" t="s">
         <v>42</v>
       </c>
@@ -9349,7 +9349,7 @@
       <c r="K55" s="204"/>
       <c r="L55" s="27"/>
     </row>
-    <row r="56" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="56" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="41" t="s">
         <v>43</v>
       </c>
@@ -9369,7 +9369,7 @@
       <c r="K56" s="205"/>
       <c r="L56" s="27"/>
     </row>
-    <row r="57" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1">
+    <row r="57" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="30"/>
       <c r="C57" s="31"/>
       <c r="D57" s="32"/>
@@ -9382,7 +9382,7 @@
       <c r="K57" s="27"/>
       <c r="L57" s="27"/>
     </row>
-    <row r="58" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="58" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="30"/>
       <c r="C58" s="31"/>
       <c r="D58" s="32"/>
@@ -9395,7 +9395,7 @@
       <c r="K58" s="27"/>
       <c r="L58" s="27"/>
     </row>
-    <row r="59" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="59" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="30"/>
       <c r="C59" s="31"/>
       <c r="D59" s="32"/>
@@ -9408,7 +9408,7 @@
       <c r="K59" s="27"/>
       <c r="L59" s="27"/>
     </row>
-    <row r="60" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="60" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="129" t="s">
         <v>170</v>
       </c>
@@ -9423,7 +9423,7 @@
       <c r="K60" s="27"/>
       <c r="L60" s="27"/>
     </row>
-    <row r="61" spans="2:12" s="28" customFormat="1" ht="65.099999999999994" customHeight="1">
+    <row r="61" spans="2:12" s="28" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="172" t="s">
         <v>134</v>
       </c>
@@ -9456,7 +9456,7 @@
       </c>
       <c r="L61" s="27"/>
     </row>
-    <row r="62" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="62" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="41" t="s">
         <v>17</v>
       </c>
@@ -9473,7 +9473,7 @@
       <c r="K62" s="204"/>
       <c r="L62" s="27"/>
     </row>
-    <row r="63" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="63" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="41" t="s">
         <v>25</v>
       </c>
@@ -9493,7 +9493,7 @@
       <c r="K63" s="205"/>
       <c r="L63" s="27"/>
     </row>
-    <row r="64" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="64" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="41" t="s">
         <v>26</v>
       </c>
@@ -9510,7 +9510,7 @@
       <c r="K64" s="204"/>
       <c r="L64" s="27"/>
     </row>
-    <row r="65" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="65" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="41" t="s">
         <v>27</v>
       </c>
@@ -9530,7 +9530,7 @@
       <c r="K65" s="205"/>
       <c r="L65" s="27"/>
     </row>
-    <row r="66" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="66" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="41" t="s">
         <v>28</v>
       </c>
@@ -9547,7 +9547,7 @@
       <c r="K66" s="204"/>
       <c r="L66" s="27"/>
     </row>
-    <row r="67" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="67" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="41" t="s">
         <v>29</v>
       </c>
@@ -9567,7 +9567,7 @@
       <c r="K67" s="205"/>
       <c r="L67" s="27"/>
     </row>
-    <row r="68" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="68" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="41" t="s">
         <v>30</v>
       </c>
@@ -9584,7 +9584,7 @@
       <c r="K68" s="204"/>
       <c r="L68" s="27"/>
     </row>
-    <row r="69" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="69" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="41" t="s">
         <v>31</v>
       </c>
@@ -9604,7 +9604,7 @@
       <c r="K69" s="205"/>
       <c r="L69" s="27"/>
     </row>
-    <row r="70" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="70" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="41" t="s">
         <v>32</v>
       </c>
@@ -9621,7 +9621,7 @@
       <c r="K70" s="204"/>
       <c r="L70" s="27"/>
     </row>
-    <row r="71" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="71" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="41" t="s">
         <v>33</v>
       </c>
@@ -9641,7 +9641,7 @@
       <c r="K71" s="205"/>
       <c r="L71" s="27"/>
     </row>
-    <row r="72" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="72" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="30"/>
       <c r="C72" s="31"/>
       <c r="D72" s="32"/>
@@ -9654,7 +9654,7 @@
       <c r="K72" s="27"/>
       <c r="L72" s="27"/>
     </row>
-    <row r="73" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="73" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="30"/>
       <c r="C73" s="31"/>
       <c r="D73" s="32"/>
@@ -9667,7 +9667,7 @@
       <c r="K73" s="27"/>
       <c r="L73" s="27"/>
     </row>
-    <row r="74" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1">
+    <row r="74" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="30"/>
       <c r="C74" s="31"/>
       <c r="D74" s="32"/>
@@ -9680,7 +9680,7 @@
       <c r="K74" s="27"/>
       <c r="L74" s="27"/>
     </row>
-    <row r="75" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1">
+    <row r="75" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="30"/>
       <c r="C75" s="31"/>
       <c r="D75" s="32"/>
@@ -9693,7 +9693,7 @@
       <c r="K75" s="27"/>
       <c r="L75" s="27"/>
     </row>
-    <row r="76" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1">
+    <row r="76" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="30"/>
       <c r="C76" s="31"/>
       <c r="D76" s="32"/>
@@ -9706,7 +9706,7 @@
       <c r="K76" s="27"/>
       <c r="L76" s="27"/>
     </row>
-    <row r="77" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="77" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="187" t="s">
         <v>163</v>
       </c>
@@ -9721,7 +9721,7 @@
       <c r="K77" s="27"/>
       <c r="L77" s="27"/>
     </row>
-    <row r="78" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="78" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="187" t="s">
         <v>150</v>
       </c>
@@ -9733,7 +9733,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="8"/>
     </row>
-    <row r="79" spans="2:12" s="19" customFormat="1" ht="62.65" customHeight="1">
+    <row r="79" spans="2:12" s="19" customFormat="1" ht="62.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="185" t="s">
         <v>14</v>
       </c>
@@ -9765,7 +9765,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="80" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="41" t="s">
         <v>17</v>
       </c>
@@ -9781,7 +9781,7 @@
       <c r="J80" s="174"/>
       <c r="K80" s="204"/>
     </row>
-    <row r="81" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="81" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="41" t="s">
         <v>25</v>
       </c>
@@ -9800,7 +9800,7 @@
       <c r="J81" s="174"/>
       <c r="K81" s="205"/>
     </row>
-    <row r="82" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="82" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="41" t="s">
         <v>26</v>
       </c>
@@ -9816,7 +9816,7 @@
       <c r="J82" s="174"/>
       <c r="K82" s="204"/>
     </row>
-    <row r="83" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="83" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="41" t="s">
         <v>27</v>
       </c>
@@ -9835,7 +9835,7 @@
       <c r="J83" s="174"/>
       <c r="K83" s="205"/>
     </row>
-    <row r="84" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="84" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="41" t="s">
         <v>28</v>
       </c>
@@ -9851,7 +9851,7 @@
       <c r="J84" s="174"/>
       <c r="K84" s="204"/>
     </row>
-    <row r="85" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="85" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="41" t="s">
         <v>29</v>
       </c>
@@ -9870,7 +9870,7 @@
       <c r="J85" s="174"/>
       <c r="K85" s="205"/>
     </row>
-    <row r="86" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="86" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="41" t="s">
         <v>30</v>
       </c>
@@ -9886,7 +9886,7 @@
       <c r="J86" s="174"/>
       <c r="K86" s="204"/>
     </row>
-    <row r="87" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="87" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="41" t="s">
         <v>31</v>
       </c>
@@ -9905,7 +9905,7 @@
       <c r="J87" s="174"/>
       <c r="K87" s="205"/>
     </row>
-    <row r="88" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="88" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="41" t="s">
         <v>32</v>
       </c>
@@ -9921,7 +9921,7 @@
       <c r="J88" s="174"/>
       <c r="K88" s="204"/>
     </row>
-    <row r="89" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="89" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="41" t="s">
         <v>33</v>
       </c>
@@ -9940,7 +9940,7 @@
       <c r="J89" s="174"/>
       <c r="K89" s="205"/>
     </row>
-    <row r="90" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="90" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="30"/>
       <c r="C90" s="31"/>
       <c r="D90" s="32"/>
@@ -9953,7 +9953,7 @@
       <c r="K90" s="27"/>
       <c r="L90" s="27"/>
     </row>
-    <row r="91" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="91" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="188"/>
       <c r="C91" s="31"/>
       <c r="D91" s="32"/>
@@ -9969,7 +9969,7 @@
       </c>
       <c r="L91" s="27"/>
     </row>
-    <row r="92" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="92" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="188"/>
       <c r="C92" s="31"/>
       <c r="D92" s="32"/>
@@ -9982,20 +9982,20 @@
       <c r="K92" s="27"/>
       <c r="L92" s="27"/>
     </row>
-    <row r="93" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="93" spans="2:12" s="28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="30"/>
       <c r="C93" s="31"/>
       <c r="D93" s="32"/>
       <c r="E93" s="23"/>
       <c r="F93" s="33"/>
-      <c r="G93" s="216"/>
-      <c r="H93" s="217"/>
+      <c r="G93" s="219"/>
+      <c r="H93" s="220"/>
       <c r="I93" s="29"/>
       <c r="J93" s="27"/>
       <c r="K93" s="27"/>
       <c r="L93" s="27"/>
     </row>
-    <row r="94" spans="2:12" ht="19.899999999999999" customHeight="1">
+    <row r="94" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="129" t="s">
         <v>149</v>
       </c>
@@ -10004,7 +10004,7 @@
       <c r="E94" s="23"/>
       <c r="F94" s="24"/>
     </row>
-    <row r="95" spans="2:12" s="16" customFormat="1" ht="72.75" customHeight="1">
+    <row r="95" spans="2:12" s="16" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="185" t="s">
         <v>14</v>
       </c>
@@ -10037,7 +10037,7 @@
       </c>
       <c r="L95" s="26"/>
     </row>
-    <row r="96" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="96" spans="2:12" s="19" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="41" t="s">
         <v>17</v>
       </c>
@@ -10054,7 +10054,7 @@
       <c r="K96" s="204"/>
       <c r="L96" s="27"/>
     </row>
-    <row r="97" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="97" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="41" t="s">
         <v>25</v>
       </c>
@@ -10074,7 +10074,7 @@
       <c r="K97" s="205"/>
       <c r="L97" s="27"/>
     </row>
-    <row r="98" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="98" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="41" t="s">
         <v>26</v>
       </c>
@@ -10091,7 +10091,7 @@
       <c r="K98" s="204"/>
       <c r="L98" s="27"/>
     </row>
-    <row r="99" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="99" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="41" t="s">
         <v>27</v>
       </c>
@@ -10111,7 +10111,7 @@
       <c r="K99" s="205"/>
       <c r="L99" s="27"/>
     </row>
-    <row r="100" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="100" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="41" t="s">
         <v>28</v>
       </c>
@@ -10128,7 +10128,7 @@
       <c r="K100" s="204"/>
       <c r="L100" s="27"/>
     </row>
-    <row r="101" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="101" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="41" t="s">
         <v>29</v>
       </c>
@@ -10148,7 +10148,7 @@
       <c r="K101" s="205"/>
       <c r="L101" s="27"/>
     </row>
-    <row r="102" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="102" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="41" t="s">
         <v>30</v>
       </c>
@@ -10165,7 +10165,7 @@
       <c r="K102" s="204"/>
       <c r="L102" s="27"/>
     </row>
-    <row r="103" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="103" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="41" t="s">
         <v>31</v>
       </c>
@@ -10185,7 +10185,7 @@
       <c r="K103" s="205"/>
       <c r="L103" s="27"/>
     </row>
-    <row r="104" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="104" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="41" t="s">
         <v>32</v>
       </c>
@@ -10202,7 +10202,7 @@
       <c r="K104" s="204"/>
       <c r="L104" s="27"/>
     </row>
-    <row r="105" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="105" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="41" t="s">
         <v>33</v>
       </c>
@@ -10222,7 +10222,7 @@
       <c r="K105" s="205"/>
       <c r="L105" s="27"/>
     </row>
-    <row r="106" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="106" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="30"/>
       <c r="C106" s="31"/>
       <c r="D106" s="32"/>
@@ -10235,7 +10235,7 @@
       <c r="K106" s="27"/>
       <c r="L106" s="27"/>
     </row>
-    <row r="107" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="107" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="129" t="s">
         <v>170</v>
       </c>
@@ -10250,7 +10250,7 @@
       <c r="K107" s="27"/>
       <c r="L107" s="27"/>
     </row>
-    <row r="108" spans="2:12" s="179" customFormat="1" ht="65.099999999999994" customHeight="1">
+    <row r="108" spans="2:12" s="179" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="172" t="s">
         <v>134</v>
       </c>
@@ -10283,7 +10283,7 @@
       </c>
       <c r="L108" s="27"/>
     </row>
-    <row r="109" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="109" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="41" t="s">
         <v>17</v>
       </c>
@@ -10300,7 +10300,7 @@
       <c r="K109" s="204"/>
       <c r="L109" s="27"/>
     </row>
-    <row r="110" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="110" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="41" t="s">
         <v>25</v>
       </c>
@@ -10320,7 +10320,7 @@
       <c r="K110" s="205"/>
       <c r="L110" s="27"/>
     </row>
-    <row r="111" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="111" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="41" t="s">
         <v>26</v>
       </c>
@@ -10337,7 +10337,7 @@
       <c r="K111" s="204"/>
       <c r="L111" s="27"/>
     </row>
-    <row r="112" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="112" spans="2:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="41" t="s">
         <v>27</v>
       </c>
@@ -10357,7 +10357,7 @@
       <c r="K112" s="205"/>
       <c r="L112" s="27"/>
     </row>
-    <row r="113" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="113" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="41" t="s">
         <v>28</v>
       </c>
@@ -10374,7 +10374,7 @@
       <c r="K113" s="204"/>
       <c r="L113" s="27"/>
     </row>
-    <row r="114" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="114" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="41" t="s">
         <v>29</v>
       </c>
@@ -10394,7 +10394,7 @@
       <c r="K114" s="205"/>
       <c r="L114" s="27"/>
     </row>
-    <row r="115" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="115" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="41" t="s">
         <v>30</v>
       </c>
@@ -10411,7 +10411,7 @@
       <c r="K115" s="204"/>
       <c r="L115" s="27"/>
     </row>
-    <row r="116" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="116" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="41" t="s">
         <v>31</v>
       </c>
@@ -10431,7 +10431,7 @@
       <c r="K116" s="205"/>
       <c r="L116" s="27"/>
     </row>
-    <row r="117" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="117" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="41" t="s">
         <v>32</v>
       </c>
@@ -10448,7 +10448,7 @@
       <c r="K117" s="204"/>
       <c r="L117" s="27"/>
     </row>
-    <row r="118" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="118" spans="1:12" s="179" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="41" t="s">
         <v>33</v>
       </c>
@@ -10468,7 +10468,7 @@
       <c r="K118" s="205"/>
       <c r="L118" s="27"/>
     </row>
-    <row r="119" spans="1:12" ht="19.899999999999999" customHeight="1">
+    <row r="119" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="30"/>
       <c r="C119" s="23"/>
@@ -10477,7 +10477,7 @@
       <c r="F119" s="23"/>
       <c r="G119" s="35"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="120" spans="1:12" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="36" t="s">
         <v>16</v>
       </c>
@@ -10492,7 +10492,7 @@
       <c r="H120" s="38"/>
       <c r="I120" s="39"/>
     </row>
-    <row r="121" spans="1:12" ht="19.899999999999999" customHeight="1">
+    <row r="121" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="34" t="s">
         <v>8</v>
       </c>
@@ -10507,21 +10507,21 @@
       <c r="H121" s="38"/>
       <c r="I121" s="1"/>
     </row>
-    <row r="122" spans="1:12" ht="40.35" customHeight="1">
-      <c r="B122" s="218" t="s">
+    <row r="122" spans="1:12" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="221" t="s">
         <v>164</v>
       </c>
-      <c r="C122" s="218"/>
-      <c r="D122" s="218"/>
-      <c r="E122" s="218"/>
-      <c r="F122" s="218"/>
-      <c r="G122" s="218"/>
-      <c r="H122" s="218"/>
-      <c r="I122" s="218"/>
-      <c r="J122" s="218"/>
-      <c r="K122" s="218"/>
-    </row>
-    <row r="123" spans="1:12" s="69" customFormat="1" ht="20.25">
+      <c r="C122" s="221"/>
+      <c r="D122" s="221"/>
+      <c r="E122" s="221"/>
+      <c r="F122" s="221"/>
+      <c r="G122" s="221"/>
+      <c r="H122" s="221"/>
+      <c r="I122" s="221"/>
+      <c r="J122" s="221"/>
+      <c r="K122" s="221"/>
+    </row>
+    <row r="123" spans="1:12" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A123" s="62"/>
       <c r="B123" s="131" t="s">
         <v>44</v>
@@ -10532,56 +10532,56 @@
       <c r="F123" s="115"/>
       <c r="H123" s="112"/>
     </row>
-    <row r="124" spans="1:12" s="69" customFormat="1" ht="20.25">
+    <row r="124" spans="1:12" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A124" s="62">
         <v>2</v>
       </c>
-      <c r="B124" s="212" t="s">
-        <v>178</v>
-      </c>
-      <c r="C124" s="212"/>
-      <c r="D124" s="212"/>
-      <c r="E124" s="212"/>
-      <c r="F124" s="212"/>
-      <c r="G124" s="212"/>
-      <c r="H124" s="212"/>
-      <c r="I124" s="212"/>
-      <c r="J124" s="212"/>
-      <c r="K124" s="212"/>
-    </row>
-    <row r="125" spans="1:12" s="69" customFormat="1" ht="20.25">
+      <c r="B124" s="222" t="s">
+        <v>177</v>
+      </c>
+      <c r="C124" s="222"/>
+      <c r="D124" s="222"/>
+      <c r="E124" s="222"/>
+      <c r="F124" s="222"/>
+      <c r="G124" s="222"/>
+      <c r="H124" s="222"/>
+      <c r="I124" s="222"/>
+      <c r="J124" s="222"/>
+      <c r="K124" s="222"/>
+    </row>
+    <row r="125" spans="1:12" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A125" s="62"/>
-      <c r="B125" s="211" t="s">
+      <c r="B125" s="223" t="s">
         <v>135</v>
       </c>
-      <c r="C125" s="211"/>
-      <c r="D125" s="211"/>
-      <c r="E125" s="211"/>
-      <c r="F125" s="211"/>
-      <c r="G125" s="211"/>
-      <c r="H125" s="211"/>
-      <c r="I125" s="211"/>
-      <c r="J125" s="211"/>
-      <c r="K125" s="211"/>
-    </row>
-    <row r="126" spans="1:12" s="69" customFormat="1" ht="20.25">
+      <c r="C125" s="223"/>
+      <c r="D125" s="223"/>
+      <c r="E125" s="223"/>
+      <c r="F125" s="223"/>
+      <c r="G125" s="223"/>
+      <c r="H125" s="223"/>
+      <c r="I125" s="223"/>
+      <c r="J125" s="223"/>
+      <c r="K125" s="223"/>
+    </row>
+    <row r="126" spans="1:12" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A126" s="62">
         <v>2</v>
       </c>
-      <c r="B126" s="212" t="s">
-        <v>179</v>
-      </c>
-      <c r="C126" s="212"/>
-      <c r="D126" s="212"/>
-      <c r="E126" s="212"/>
-      <c r="F126" s="212"/>
-      <c r="G126" s="212"/>
-      <c r="H126" s="212"/>
-      <c r="I126" s="212"/>
-      <c r="J126" s="212"/>
-      <c r="K126" s="212"/>
-    </row>
-    <row r="127" spans="1:12" ht="19.899999999999999" customHeight="1">
+      <c r="B126" s="222" t="s">
+        <v>178</v>
+      </c>
+      <c r="C126" s="222"/>
+      <c r="D126" s="222"/>
+      <c r="E126" s="222"/>
+      <c r="F126" s="222"/>
+      <c r="G126" s="222"/>
+      <c r="H126" s="222"/>
+      <c r="I126" s="222"/>
+      <c r="J126" s="222"/>
+      <c r="K126" s="222"/>
+    </row>
+    <row r="127" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="34" t="s">
         <v>8</v>
       </c>
@@ -10596,24 +10596,24 @@
       <c r="H127" s="38"/>
       <c r="I127" s="1"/>
     </row>
-    <row r="128" spans="1:12" s="69" customFormat="1" ht="20.25">
+    <row r="128" spans="1:12" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A128" s="62">
         <v>3</v>
       </c>
-      <c r="B128" s="212" t="s">
-        <v>180</v>
-      </c>
-      <c r="C128" s="212"/>
-      <c r="D128" s="212"/>
-      <c r="E128" s="212"/>
-      <c r="F128" s="212"/>
-      <c r="G128" s="212"/>
-      <c r="H128" s="212"/>
-      <c r="I128" s="212"/>
-      <c r="J128" s="212"/>
-      <c r="K128" s="212"/>
-    </row>
-    <row r="129" spans="1:11" ht="19.899999999999999" customHeight="1">
+      <c r="B128" s="222" t="s">
+        <v>179</v>
+      </c>
+      <c r="C128" s="222"/>
+      <c r="D128" s="222"/>
+      <c r="E128" s="222"/>
+      <c r="F128" s="222"/>
+      <c r="G128" s="222"/>
+      <c r="H128" s="222"/>
+      <c r="I128" s="222"/>
+      <c r="J128" s="222"/>
+      <c r="K128" s="222"/>
+    </row>
+    <row r="129" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="34" t="s">
         <v>8</v>
       </c>
@@ -10628,24 +10628,24 @@
       <c r="H129" s="38"/>
       <c r="I129" s="1"/>
     </row>
-    <row r="130" spans="1:11" s="69" customFormat="1" ht="20.25">
+    <row r="130" spans="1:11" s="69" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A130" s="62">
         <v>3</v>
       </c>
-      <c r="B130" s="212" t="s">
-        <v>181</v>
-      </c>
-      <c r="C130" s="212"/>
-      <c r="D130" s="212"/>
-      <c r="E130" s="212"/>
-      <c r="F130" s="212"/>
-      <c r="G130" s="212"/>
-      <c r="H130" s="212"/>
-      <c r="I130" s="212"/>
-      <c r="J130" s="212"/>
-      <c r="K130" s="212"/>
-    </row>
-    <row r="132" spans="1:11" s="69" customFormat="1" ht="33.200000000000003" customHeight="1">
+      <c r="B130" s="222" t="s">
+        <v>180</v>
+      </c>
+      <c r="C130" s="222"/>
+      <c r="D130" s="222"/>
+      <c r="E130" s="222"/>
+      <c r="F130" s="222"/>
+      <c r="G130" s="222"/>
+      <c r="H130" s="222"/>
+      <c r="I130" s="222"/>
+      <c r="J130" s="222"/>
+      <c r="K130" s="222"/>
+    </row>
+    <row r="132" spans="1:11" s="69" customFormat="1" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="62"/>
       <c r="B132" s="4" t="s">
         <v>10</v>
@@ -10660,33 +10660,21 @@
       <c r="J132" s="6"/>
       <c r="K132" s="6"/>
     </row>
-    <row r="133" spans="1:11" ht="26.25" customHeight="1"/>
-    <row r="134" spans="1:11" ht="26.25" customHeight="1"/>
-    <row r="135" spans="1:11" ht="42" customHeight="1"/>
+    <row r="133" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B124:K124"/>
+    <mergeCell ref="B125:K125"/>
+    <mergeCell ref="B126:K126"/>
+    <mergeCell ref="B128:K128"/>
+    <mergeCell ref="B130:K130"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B122:K122"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="C15:D15"/>
@@ -10695,16 +10683,28 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B122:K122"/>
-    <mergeCell ref="B124:K124"/>
-    <mergeCell ref="B125:K125"/>
-    <mergeCell ref="B126:K126"/>
-    <mergeCell ref="B128:K128"/>
-    <mergeCell ref="B130:K130"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B9">
@@ -10813,7 +10813,7 @@
       <selection pane="bottomRight" activeCell="S3" sqref="S3:S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="133" customWidth="1"/>
     <col min="2" max="2" width="16.125" style="133" customWidth="1"/>
@@ -10833,32 +10833,32 @@
     <col min="38" max="16384" width="8.875" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="42.75" customHeight="1">
+    <row r="1" spans="1:37" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="152"/>
       <c r="B1" s="152"/>
-      <c r="U1" s="222" t="s">
+      <c r="U1" s="224" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="222"/>
-      <c r="W1" s="222"/>
-      <c r="X1" s="222"/>
-      <c r="Y1" s="222"/>
-      <c r="Z1" s="222"/>
-      <c r="AA1" s="222"/>
-      <c r="AB1" s="222" t="s">
+      <c r="V1" s="224"/>
+      <c r="W1" s="224"/>
+      <c r="X1" s="224"/>
+      <c r="Y1" s="224"/>
+      <c r="Z1" s="224"/>
+      <c r="AA1" s="224"/>
+      <c r="AB1" s="224" t="s">
         <v>59</v>
       </c>
-      <c r="AC1" s="222"/>
-      <c r="AD1" s="222"/>
-      <c r="AE1" s="222"/>
-      <c r="AF1" s="222"/>
-      <c r="AG1" s="222"/>
-      <c r="AH1" s="222"/>
-      <c r="AI1" s="222"/>
-      <c r="AJ1" s="222"/>
-      <c r="AK1" s="222"/>
-    </row>
-    <row r="2" spans="1:37" ht="78">
+      <c r="AC1" s="224"/>
+      <c r="AD1" s="224"/>
+      <c r="AE1" s="224"/>
+      <c r="AF1" s="224"/>
+      <c r="AG1" s="224"/>
+      <c r="AH1" s="224"/>
+      <c r="AI1" s="224"/>
+      <c r="AJ1" s="224"/>
+      <c r="AK1" s="224"/>
+    </row>
+    <row r="2" spans="1:37" ht="78" x14ac:dyDescent="0.25">
       <c r="A2" s="162" t="s">
         <v>106</v>
       </c>
@@ -10971,7 +10971,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="18" customHeight="1">
+    <row r="3" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="134"/>
       <c r="B3" s="134"/>
       <c r="C3" s="138"/>
@@ -11010,7 +11010,7 @@
       <c r="AJ3" s="145"/>
       <c r="AK3" s="145"/>
     </row>
-    <row r="4" spans="1:37" ht="18" customHeight="1">
+    <row r="4" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="134"/>
       <c r="B4" s="134"/>
       <c r="C4" s="138"/>
@@ -11049,7 +11049,7 @@
       <c r="AJ4" s="145"/>
       <c r="AK4" s="145"/>
     </row>
-    <row r="5" spans="1:37" ht="18" customHeight="1">
+    <row r="5" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="134"/>
       <c r="B5" s="134"/>
       <c r="C5" s="138"/>
@@ -11088,7 +11088,7 @@
       <c r="AJ5" s="145"/>
       <c r="AK5" s="145"/>
     </row>
-    <row r="6" spans="1:37" ht="18" customHeight="1">
+    <row r="6" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="134"/>
       <c r="B6" s="134"/>
       <c r="C6" s="138"/>
@@ -11127,7 +11127,7 @@
       <c r="AJ6" s="145"/>
       <c r="AK6" s="145"/>
     </row>
-    <row r="7" spans="1:37" ht="18" customHeight="1">
+    <row r="7" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="134"/>
       <c r="B7" s="134"/>
       <c r="C7" s="138"/>
@@ -11166,7 +11166,7 @@
       <c r="AJ7" s="145"/>
       <c r="AK7" s="145"/>
     </row>
-    <row r="8" spans="1:37" ht="18" customHeight="1">
+    <row r="8" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="134"/>
       <c r="B8" s="134"/>
       <c r="C8" s="138"/>
@@ -11205,7 +11205,7 @@
       <c r="AJ8" s="145"/>
       <c r="AK8" s="145"/>
     </row>
-    <row r="9" spans="1:37" ht="18" customHeight="1">
+    <row r="9" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="134"/>
       <c r="B9" s="134"/>
       <c r="C9" s="138"/>
@@ -11244,7 +11244,7 @@
       <c r="AJ9" s="145"/>
       <c r="AK9" s="145"/>
     </row>
-    <row r="10" spans="1:37" ht="18" customHeight="1">
+    <row r="10" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="134"/>
       <c r="B10" s="134"/>
       <c r="C10" s="138"/>
@@ -11283,7 +11283,7 @@
       <c r="AJ10" s="145"/>
       <c r="AK10" s="145"/>
     </row>
-    <row r="11" spans="1:37" ht="18" customHeight="1">
+    <row r="11" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="134"/>
       <c r="B11" s="134"/>
       <c r="C11" s="138"/>
@@ -11322,7 +11322,7 @@
       <c r="AJ11" s="145"/>
       <c r="AK11" s="145"/>
     </row>
-    <row r="12" spans="1:37" ht="18" customHeight="1">
+    <row r="12" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="134"/>
       <c r="B12" s="134"/>
       <c r="C12" s="138"/>
@@ -11361,7 +11361,7 @@
       <c r="AJ12" s="145"/>
       <c r="AK12" s="145"/>
     </row>
-    <row r="13" spans="1:37" ht="18" customHeight="1">
+    <row r="13" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="134"/>
       <c r="B13" s="134"/>
       <c r="C13" s="138"/>
@@ -11400,7 +11400,7 @@
       <c r="AJ13" s="145"/>
       <c r="AK13" s="145"/>
     </row>
-    <row r="14" spans="1:37" ht="18" customHeight="1">
+    <row r="14" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="134"/>
       <c r="B14" s="134"/>
       <c r="C14" s="138"/>
@@ -11439,7 +11439,7 @@
       <c r="AJ14" s="145"/>
       <c r="AK14" s="145"/>
     </row>
-    <row r="15" spans="1:37" ht="18" customHeight="1">
+    <row r="15" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="134"/>
       <c r="B15" s="134"/>
       <c r="C15" s="138"/>
@@ -11478,7 +11478,7 @@
       <c r="AJ15" s="145"/>
       <c r="AK15" s="145"/>
     </row>
-    <row r="16" spans="1:37" ht="18" customHeight="1">
+    <row r="16" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="134"/>
       <c r="B16" s="134"/>
       <c r="C16" s="138"/>
@@ -11517,7 +11517,7 @@
       <c r="AJ16" s="145"/>
       <c r="AK16" s="145"/>
     </row>
-    <row r="17" spans="1:37" ht="18" customHeight="1">
+    <row r="17" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="134"/>
       <c r="B17" s="134"/>
       <c r="C17" s="138"/>
@@ -11556,7 +11556,7 @@
       <c r="AJ17" s="145"/>
       <c r="AK17" s="145"/>
     </row>
-    <row r="18" spans="1:37" ht="18" customHeight="1">
+    <row r="18" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="134"/>
       <c r="B18" s="134"/>
       <c r="C18" s="138"/>
@@ -11595,7 +11595,7 @@
       <c r="AJ18" s="145"/>
       <c r="AK18" s="145"/>
     </row>
-    <row r="19" spans="1:37" ht="18" customHeight="1">
+    <row r="19" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="134"/>
       <c r="B19" s="134"/>
       <c r="C19" s="138"/>
@@ -11634,7 +11634,7 @@
       <c r="AJ19" s="145"/>
       <c r="AK19" s="145"/>
     </row>
-    <row r="20" spans="1:37" ht="18" customHeight="1">
+    <row r="20" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="134"/>
       <c r="B20" s="134"/>
       <c r="C20" s="138"/>
@@ -11673,7 +11673,7 @@
       <c r="AJ20" s="145"/>
       <c r="AK20" s="145"/>
     </row>
-    <row r="21" spans="1:37" ht="18" customHeight="1">
+    <row r="21" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="134"/>
       <c r="B21" s="134"/>
       <c r="C21" s="138"/>
@@ -11712,7 +11712,7 @@
       <c r="AJ21" s="145"/>
       <c r="AK21" s="145"/>
     </row>
-    <row r="22" spans="1:37" ht="18" customHeight="1">
+    <row r="22" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="134"/>
       <c r="B22" s="134"/>
       <c r="C22" s="138"/>
@@ -11751,7 +11751,7 @@
       <c r="AJ22" s="145"/>
       <c r="AK22" s="145"/>
     </row>
-    <row r="23" spans="1:37" ht="18" customHeight="1">
+    <row r="23" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="134"/>
       <c r="B23" s="134"/>
       <c r="C23" s="138"/>
@@ -11790,7 +11790,7 @@
       <c r="AJ23" s="145"/>
       <c r="AK23" s="145"/>
     </row>
-    <row r="24" spans="1:37" ht="18" customHeight="1">
+    <row r="24" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="134"/>
       <c r="B24" s="134"/>
       <c r="C24" s="138"/>
@@ -11829,7 +11829,7 @@
       <c r="AJ24" s="145"/>
       <c r="AK24" s="145"/>
     </row>
-    <row r="25" spans="1:37" ht="18" customHeight="1">
+    <row r="25" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="134"/>
       <c r="B25" s="134"/>
       <c r="C25" s="138"/>
@@ -11868,7 +11868,7 @@
       <c r="AJ25" s="145"/>
       <c r="AK25" s="145"/>
     </row>
-    <row r="26" spans="1:37" ht="18" customHeight="1">
+    <row r="26" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="134"/>
       <c r="B26" s="134"/>
       <c r="C26" s="138"/>
@@ -11907,7 +11907,7 @@
       <c r="AJ26" s="145"/>
       <c r="AK26" s="145"/>
     </row>
-    <row r="27" spans="1:37" ht="18" customHeight="1">
+    <row r="27" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="134"/>
       <c r="B27" s="134"/>
       <c r="C27" s="138"/>
@@ -11946,7 +11946,7 @@
       <c r="AJ27" s="145"/>
       <c r="AK27" s="145"/>
     </row>
-    <row r="28" spans="1:37" ht="18" customHeight="1">
+    <row r="28" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="134"/>
       <c r="B28" s="134"/>
       <c r="C28" s="138"/>
@@ -11985,7 +11985,7 @@
       <c r="AJ28" s="145"/>
       <c r="AK28" s="145"/>
     </row>
-    <row r="29" spans="1:37" ht="18" customHeight="1">
+    <row r="29" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="134"/>
       <c r="B29" s="134"/>
       <c r="C29" s="138"/>
@@ -12024,7 +12024,7 @@
       <c r="AJ29" s="145"/>
       <c r="AK29" s="145"/>
     </row>
-    <row r="30" spans="1:37" ht="18" customHeight="1">
+    <row r="30" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="134"/>
       <c r="B30" s="134"/>
       <c r="C30" s="138"/>
@@ -12063,10 +12063,10 @@
       <c r="AJ30" s="145"/>
       <c r="AK30" s="145"/>
     </row>
-    <row r="33" spans="2:21">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="164"/>
     </row>
-    <row r="34" spans="2:21" ht="19.5">
+    <row r="34" spans="2:21" ht="19.5" x14ac:dyDescent="0.25">
       <c r="U34" s="163" t="s">
         <v>108</v>
       </c>
@@ -12099,7 +12099,7 @@
       <selection pane="bottomRight" activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.25" customWidth="1"/>
     <col min="2" max="2" width="12.125" style="133" customWidth="1"/>
@@ -12119,31 +12119,31 @@
     <col min="35" max="37" width="11" style="147" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="133" customFormat="1" ht="42" customHeight="1">
+    <row r="1" spans="1:37" s="133" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="152"/>
-      <c r="U1" s="223" t="s">
+      <c r="U1" s="225" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="222"/>
-      <c r="W1" s="222"/>
-      <c r="X1" s="222"/>
-      <c r="Y1" s="222"/>
-      <c r="Z1" s="222"/>
-      <c r="AA1" s="222"/>
-      <c r="AB1" s="224" t="s">
+      <c r="V1" s="224"/>
+      <c r="W1" s="224"/>
+      <c r="X1" s="224"/>
+      <c r="Y1" s="224"/>
+      <c r="Z1" s="224"/>
+      <c r="AA1" s="224"/>
+      <c r="AB1" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="226"/>
-    </row>
-    <row r="2" spans="1:37" s="133" customFormat="1" ht="78">
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="228"/>
+    </row>
+    <row r="2" spans="1:37" s="133" customFormat="1" ht="78" x14ac:dyDescent="0.25">
       <c r="A2" s="162" t="s">
         <v>106</v>
       </c>
@@ -12256,7 +12256,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="3" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="134"/>
       <c r="B3" s="134"/>
       <c r="C3" s="138"/>
@@ -12295,7 +12295,7 @@
       <c r="AJ3" s="145"/>
       <c r="AK3" s="145"/>
     </row>
-    <row r="4" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="4" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="134"/>
       <c r="B4" s="134"/>
       <c r="C4" s="138"/>
@@ -12334,7 +12334,7 @@
       <c r="AJ4" s="145"/>
       <c r="AK4" s="145"/>
     </row>
-    <row r="5" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="5" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="134"/>
       <c r="B5" s="134"/>
       <c r="C5" s="138"/>
@@ -12373,7 +12373,7 @@
       <c r="AJ5" s="145"/>
       <c r="AK5" s="145"/>
     </row>
-    <row r="6" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="6" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="134"/>
       <c r="B6" s="134"/>
       <c r="C6" s="138"/>
@@ -12412,7 +12412,7 @@
       <c r="AJ6" s="145"/>
       <c r="AK6" s="145"/>
     </row>
-    <row r="7" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="134"/>
       <c r="B7" s="134"/>
       <c r="C7" s="138"/>
@@ -12451,7 +12451,7 @@
       <c r="AJ7" s="145"/>
       <c r="AK7" s="145"/>
     </row>
-    <row r="8" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="8" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="134"/>
       <c r="B8" s="134"/>
       <c r="C8" s="138"/>
@@ -12490,7 +12490,7 @@
       <c r="AJ8" s="145"/>
       <c r="AK8" s="145"/>
     </row>
-    <row r="9" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="134"/>
       <c r="B9" s="134"/>
       <c r="C9" s="138"/>
@@ -12529,7 +12529,7 @@
       <c r="AJ9" s="145"/>
       <c r="AK9" s="145"/>
     </row>
-    <row r="10" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="10" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="134"/>
       <c r="B10" s="134"/>
       <c r="C10" s="138"/>
@@ -12568,7 +12568,7 @@
       <c r="AJ10" s="145"/>
       <c r="AK10" s="145"/>
     </row>
-    <row r="11" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="11" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="134"/>
       <c r="B11" s="134"/>
       <c r="C11" s="138"/>
@@ -12607,7 +12607,7 @@
       <c r="AJ11" s="145"/>
       <c r="AK11" s="145"/>
     </row>
-    <row r="12" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="12" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="134"/>
       <c r="B12" s="134"/>
       <c r="C12" s="138"/>
@@ -12646,7 +12646,7 @@
       <c r="AJ12" s="145"/>
       <c r="AK12" s="145"/>
     </row>
-    <row r="13" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="13" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="134"/>
       <c r="B13" s="134"/>
       <c r="C13" s="138"/>
@@ -12685,7 +12685,7 @@
       <c r="AJ13" s="145"/>
       <c r="AK13" s="145"/>
     </row>
-    <row r="14" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="14" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="134"/>
       <c r="B14" s="134"/>
       <c r="C14" s="138"/>
@@ -12724,7 +12724,7 @@
       <c r="AJ14" s="145"/>
       <c r="AK14" s="145"/>
     </row>
-    <row r="15" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="15" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="134"/>
       <c r="B15" s="134"/>
       <c r="C15" s="138"/>
@@ -12763,7 +12763,7 @@
       <c r="AJ15" s="145"/>
       <c r="AK15" s="145"/>
     </row>
-    <row r="16" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="16" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="134"/>
       <c r="B16" s="134"/>
       <c r="C16" s="138"/>
@@ -12802,7 +12802,7 @@
       <c r="AJ16" s="145"/>
       <c r="AK16" s="145"/>
     </row>
-    <row r="17" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="17" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="134"/>
       <c r="B17" s="134"/>
       <c r="C17" s="138"/>
@@ -12841,7 +12841,7 @@
       <c r="AJ17" s="145"/>
       <c r="AK17" s="145"/>
     </row>
-    <row r="18" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="18" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="134"/>
       <c r="B18" s="134"/>
       <c r="C18" s="138"/>
@@ -12880,7 +12880,7 @@
       <c r="AJ18" s="145"/>
       <c r="AK18" s="145"/>
     </row>
-    <row r="19" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="19" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="134"/>
       <c r="B19" s="134"/>
       <c r="C19" s="138"/>
@@ -12919,7 +12919,7 @@
       <c r="AJ19" s="145"/>
       <c r="AK19" s="145"/>
     </row>
-    <row r="20" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="20" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="134"/>
       <c r="B20" s="134"/>
       <c r="C20" s="138"/>
@@ -12958,7 +12958,7 @@
       <c r="AJ20" s="145"/>
       <c r="AK20" s="145"/>
     </row>
-    <row r="21" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="21" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="134"/>
       <c r="B21" s="134"/>
       <c r="C21" s="138"/>
@@ -12997,7 +12997,7 @@
       <c r="AJ21" s="145"/>
       <c r="AK21" s="145"/>
     </row>
-    <row r="22" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="22" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="134"/>
       <c r="B22" s="134"/>
       <c r="C22" s="138"/>
@@ -13036,7 +13036,7 @@
       <c r="AJ22" s="145"/>
       <c r="AK22" s="145"/>
     </row>
-    <row r="23" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="23" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="134"/>
       <c r="B23" s="134"/>
       <c r="C23" s="138"/>
@@ -13075,7 +13075,7 @@
       <c r="AJ23" s="145"/>
       <c r="AK23" s="145"/>
     </row>
-    <row r="24" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="24" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="134"/>
       <c r="B24" s="134"/>
       <c r="C24" s="138"/>
@@ -13114,7 +13114,7 @@
       <c r="AJ24" s="145"/>
       <c r="AK24" s="145"/>
     </row>
-    <row r="25" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="25" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="134"/>
       <c r="B25" s="134"/>
       <c r="C25" s="138"/>
@@ -13153,7 +13153,7 @@
       <c r="AJ25" s="145"/>
       <c r="AK25" s="145"/>
     </row>
-    <row r="26" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="26" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="134"/>
       <c r="B26" s="134"/>
       <c r="C26" s="138"/>
@@ -13192,7 +13192,7 @@
       <c r="AJ26" s="145"/>
       <c r="AK26" s="145"/>
     </row>
-    <row r="27" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="27" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="134"/>
       <c r="B27" s="134"/>
       <c r="C27" s="138"/>
@@ -13231,7 +13231,7 @@
       <c r="AJ27" s="145"/>
       <c r="AK27" s="145"/>
     </row>
-    <row r="28" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="28" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="134"/>
       <c r="B28" s="134"/>
       <c r="C28" s="138"/>
@@ -13270,7 +13270,7 @@
       <c r="AJ28" s="145"/>
       <c r="AK28" s="145"/>
     </row>
-    <row r="29" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="29" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="134"/>
       <c r="B29" s="134"/>
       <c r="C29" s="138"/>
@@ -13309,7 +13309,7 @@
       <c r="AJ29" s="145"/>
       <c r="AK29" s="145"/>
     </row>
-    <row r="30" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1">
+    <row r="30" spans="1:37" s="133" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="134"/>
       <c r="B30" s="134"/>
       <c r="C30" s="138"/>
@@ -13348,10 +13348,10 @@
       <c r="AJ30" s="145"/>
       <c r="AK30" s="145"/>
     </row>
-    <row r="33" spans="1:21" ht="19.5">
+    <row r="33" spans="1:21" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="163"/>
     </row>
-    <row r="34" spans="1:21" ht="19.5">
+    <row r="34" spans="1:21" ht="19.5" x14ac:dyDescent="0.25">
       <c r="U34" s="163" t="s">
         <v>108</v>
       </c>

</xml_diff>